<commit_message>
MaJ avant ajout bouton export STFs
</commit_message>
<xml_diff>
--- a/template/stf_templates.xlsx
+++ b/template/stf_templates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thomas\Desktop\Scripts\STF_Generator\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D834A2C-B7A6-42FE-9B64-25CE7F7A3DBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{380FF212-224B-4548-A052-487BE1E9C02C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0D2206E1-184A-44E3-86B4-27359D5FA673}"/>
   </bookViews>
@@ -1098,6 +1098,126 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1113,166 +1233,52 @@
     <xf numFmtId="49" fontId="4" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="2" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="2" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1281,6 +1287,12 @@
     <xf numFmtId="49" fontId="1" fillId="2" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="9" fillId="2" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="2" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1291,6 +1303,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1308,18 +1323,6 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1329,20 +1332,17 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1661,7 +1661,7 @@
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21:H21"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1676,30 +1676,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="74" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="38"/>
+      <c r="B1" s="75"/>
+      <c r="C1" s="75"/>
+      <c r="D1" s="75"/>
+      <c r="E1" s="75"/>
+      <c r="F1" s="75"/>
+      <c r="G1" s="75"/>
+      <c r="H1" s="76"/>
     </row>
     <row r="2" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="66" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="27"/>
+      <c r="B2" s="67"/>
       <c r="C2" s="16">
         <v>1</v>
       </c>
-      <c r="D2" s="28" t="s">
+      <c r="D2" s="68" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="29"/>
-      <c r="F2" s="30"/>
+      <c r="E2" s="69"/>
+      <c r="F2" s="70"/>
       <c r="G2" s="19" t="s">
         <v>28</v>
       </c>
@@ -1708,18 +1708,18 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="31" t="s">
+      <c r="A3" s="43" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="32"/>
+      <c r="B3" s="44"/>
       <c r="C3" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="33" t="s">
+      <c r="D3" s="71" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="34"/>
-      <c r="F3" s="35"/>
+      <c r="E3" s="72"/>
+      <c r="F3" s="73"/>
       <c r="G3" s="20" t="s">
         <v>53</v>
       </c>
@@ -1728,102 +1728,102 @@
       </c>
     </row>
     <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="39" t="s">
+      <c r="A4" s="61" t="s">
         <v>31</v>
       </c>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
+      <c r="B4" s="62"/>
+      <c r="C4" s="62"/>
       <c r="D4" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="E4" s="41" t="s">
+      <c r="E4" s="63" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="41"/>
-      <c r="G4" s="42" t="s">
+      <c r="F4" s="63"/>
+      <c r="G4" s="64" t="s">
         <v>46</v>
       </c>
-      <c r="H4" s="43"/>
+      <c r="H4" s="65"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="44" t="s">
+      <c r="A5" s="45" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="45"/>
-      <c r="C5" s="45"/>
+      <c r="B5" s="46"/>
+      <c r="C5" s="46"/>
       <c r="D5" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="E5" s="46" t="s">
+      <c r="E5" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="46"/>
-      <c r="G5" s="47" t="s">
+      <c r="F5" s="47"/>
+      <c r="G5" s="48" t="s">
         <v>45</v>
       </c>
-      <c r="H5" s="48"/>
+      <c r="H5" s="49"/>
     </row>
     <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="44" t="s">
+      <c r="A6" s="45" t="s">
         <v>33</v>
       </c>
-      <c r="B6" s="45"/>
-      <c r="C6" s="45"/>
+      <c r="B6" s="46"/>
+      <c r="C6" s="46"/>
       <c r="D6" s="6"/>
-      <c r="E6" s="46" t="s">
+      <c r="E6" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="F6" s="46"/>
-      <c r="G6" s="47" t="s">
+      <c r="F6" s="47"/>
+      <c r="G6" s="48" t="s">
         <v>44</v>
       </c>
-      <c r="H6" s="48"/>
+      <c r="H6" s="49"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="44" t="s">
+      <c r="A7" s="45" t="s">
         <v>34</v>
       </c>
-      <c r="B7" s="45"/>
-      <c r="C7" s="45"/>
+      <c r="B7" s="46"/>
+      <c r="C7" s="46"/>
       <c r="D7" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="E7" s="46" t="s">
+      <c r="E7" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="F7" s="46"/>
-      <c r="G7" s="47" t="s">
+      <c r="F7" s="47"/>
+      <c r="G7" s="48" t="s">
         <v>52</v>
       </c>
-      <c r="H7" s="48"/>
+      <c r="H7" s="49"/>
     </row>
     <row r="8" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="44" t="s">
+      <c r="A8" s="45" t="s">
         <v>35</v>
       </c>
-      <c r="B8" s="45"/>
-      <c r="C8" s="45"/>
+      <c r="B8" s="46"/>
+      <c r="C8" s="46"/>
       <c r="D8" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="E8" s="46" t="s">
+      <c r="E8" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="F8" s="46"/>
-      <c r="G8" s="47" t="s">
+      <c r="F8" s="47"/>
+      <c r="G8" s="48" t="s">
         <v>43</v>
       </c>
-      <c r="H8" s="48"/>
+      <c r="H8" s="49"/>
     </row>
     <row r="9" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="31" t="s">
+      <c r="A9" s="43" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="32"/>
-      <c r="C9" s="32"/>
+      <c r="B9" s="44"/>
+      <c r="C9" s="44"/>
       <c r="D9" s="2"/>
-      <c r="E9" s="49"/>
-      <c r="F9" s="49"/>
+      <c r="E9" s="34"/>
+      <c r="F9" s="34"/>
       <c r="G9" s="50"/>
       <c r="H9" s="51"/>
     </row>
@@ -1842,11 +1842,11 @@
       <c r="H10" s="57"/>
     </row>
     <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="31" t="s">
+      <c r="A11" s="43" t="s">
         <v>38</v>
       </c>
-      <c r="B11" s="32"/>
-      <c r="C11" s="32"/>
+      <c r="B11" s="44"/>
+      <c r="C11" s="44"/>
       <c r="D11" s="58"/>
       <c r="E11" s="59"/>
       <c r="F11" s="59"/>
@@ -1854,182 +1854,180 @@
       <c r="H11" s="60"/>
     </row>
     <row r="12" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="75"/>
-      <c r="B12" s="76"/>
-      <c r="C12" s="76"/>
-      <c r="D12" s="76"/>
+      <c r="A12" s="41"/>
+      <c r="B12" s="42"/>
+      <c r="C12" s="42"/>
+      <c r="D12" s="42"/>
       <c r="E12" s="8" t="s">
         <v>7</v>
       </c>
       <c r="F12" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="G12" s="61" t="s">
+      <c r="G12" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="H12" s="62"/>
+      <c r="H12" s="37"/>
     </row>
     <row r="13" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="63" t="s">
+      <c r="B13" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="63"/>
-      <c r="D13" s="63"/>
+      <c r="C13" s="38"/>
+      <c r="D13" s="38"/>
       <c r="E13" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F13" s="10"/>
-      <c r="G13" s="64"/>
-      <c r="H13" s="65"/>
+      <c r="G13" s="39"/>
+      <c r="H13" s="40"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="66" t="s">
+      <c r="B14" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="66"/>
-      <c r="D14" s="66"/>
+      <c r="C14" s="26"/>
+      <c r="D14" s="26"/>
       <c r="E14" s="7" t="s">
         <v>12</v>
       </c>
       <c r="F14" s="7"/>
-      <c r="G14" s="67"/>
-      <c r="H14" s="68"/>
+      <c r="G14" s="27"/>
+      <c r="H14" s="28"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="66" t="s">
+      <c r="B15" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="66"/>
-      <c r="D15" s="66"/>
+      <c r="C15" s="26"/>
+      <c r="D15" s="26"/>
       <c r="E15" s="7" t="s">
         <v>12</v>
       </c>
       <c r="F15" s="7"/>
-      <c r="G15" s="67"/>
-      <c r="H15" s="68"/>
+      <c r="G15" s="27"/>
+      <c r="H15" s="28"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="66" t="s">
+      <c r="B16" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="66"/>
-      <c r="D16" s="66"/>
+      <c r="C16" s="26"/>
+      <c r="D16" s="26"/>
       <c r="E16" s="7" t="s">
         <v>12</v>
       </c>
       <c r="F16" s="7"/>
-      <c r="G16" s="67"/>
-      <c r="H16" s="68"/>
+      <c r="G16" s="27"/>
+      <c r="H16" s="28"/>
     </row>
     <row r="17" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="74" t="s">
+      <c r="B17" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="C17" s="74"/>
-      <c r="D17" s="74"/>
+      <c r="C17" s="29"/>
+      <c r="D17" s="29"/>
       <c r="E17" s="12" t="s">
         <v>40</v>
       </c>
       <c r="F17" s="7"/>
-      <c r="G17" s="67"/>
-      <c r="H17" s="68"/>
+      <c r="G17" s="27"/>
+      <c r="H17" s="28"/>
     </row>
     <row r="18" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="B18" s="66" t="s">
+      <c r="B18" s="26" t="s">
         <v>80</v>
       </c>
-      <c r="C18" s="66"/>
-      <c r="D18" s="66"/>
+      <c r="C18" s="26"/>
+      <c r="D18" s="26"/>
       <c r="E18" s="12" t="s">
         <v>39</v>
       </c>
       <c r="F18" s="7"/>
-      <c r="G18" s="67"/>
-      <c r="H18" s="68"/>
+      <c r="G18" s="27"/>
+      <c r="H18" s="28"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="66" t="s">
+      <c r="B19" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="C19" s="66"/>
-      <c r="D19" s="66"/>
+      <c r="C19" s="26"/>
+      <c r="D19" s="26"/>
       <c r="E19" s="7" t="s">
         <v>12</v>
       </c>
       <c r="F19" s="7"/>
-      <c r="G19" s="67"/>
-      <c r="H19" s="68"/>
+      <c r="G19" s="27"/>
+      <c r="H19" s="28"/>
     </row>
     <row r="20" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B20" s="72" t="s">
+      <c r="B20" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="C20" s="72"/>
-      <c r="D20" s="72"/>
+      <c r="C20" s="33"/>
+      <c r="D20" s="33"/>
       <c r="E20" s="14" t="s">
         <v>41</v>
       </c>
       <c r="F20" s="15"/>
-      <c r="G20" s="49"/>
-      <c r="H20" s="73"/>
+      <c r="G20" s="34"/>
+      <c r="H20" s="35"/>
     </row>
     <row r="21" spans="1:8" s="18" customFormat="1" ht="92.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="69" t="s">
+      <c r="A21" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="B21" s="70"/>
-      <c r="C21" s="70"/>
-      <c r="D21" s="70"/>
-      <c r="E21" s="70"/>
-      <c r="F21" s="70"/>
-      <c r="G21" s="70"/>
-      <c r="H21" s="71"/>
+      <c r="B21" s="31"/>
+      <c r="C21" s="31"/>
+      <c r="D21" s="31"/>
+      <c r="E21" s="31"/>
+      <c r="F21" s="31"/>
+      <c r="G21" s="31"/>
+      <c r="H21" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="47">
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="A21:H21"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="A12:D12"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="G7:H7"/>
     <mergeCell ref="A11:C11"/>
     <mergeCell ref="A8:C8"/>
     <mergeCell ref="E8:F8"/>
@@ -2041,23 +2039,25 @@
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="G10:H10"/>
     <mergeCell ref="D11:H11"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="A12:D12"/>
+    <mergeCell ref="A21:H21"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="G17:H17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2069,7 +2069,7 @@
   <dimension ref="A1:H43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2084,30 +2084,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="74" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="38"/>
+      <c r="B1" s="75"/>
+      <c r="C1" s="75"/>
+      <c r="D1" s="75"/>
+      <c r="E1" s="75"/>
+      <c r="F1" s="75"/>
+      <c r="G1" s="75"/>
+      <c r="H1" s="76"/>
     </row>
     <row r="2" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="66" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="27"/>
+      <c r="B2" s="67"/>
       <c r="C2" s="16">
         <v>1</v>
       </c>
-      <c r="D2" s="28" t="s">
+      <c r="D2" s="68" t="s">
         <v>54</v>
       </c>
-      <c r="E2" s="29"/>
-      <c r="F2" s="30"/>
+      <c r="E2" s="69"/>
+      <c r="F2" s="70"/>
       <c r="G2" s="19" t="s">
         <v>28</v>
       </c>
@@ -2116,18 +2116,18 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="31" t="s">
+      <c r="A3" s="43" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="32"/>
+      <c r="B3" s="44"/>
       <c r="C3" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="33" t="s">
+      <c r="D3" s="71" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="34"/>
-      <c r="F3" s="35"/>
+      <c r="E3" s="72"/>
+      <c r="F3" s="73"/>
       <c r="G3" s="20" t="s">
         <v>53</v>
       </c>
@@ -2136,125 +2136,125 @@
       </c>
     </row>
     <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="39" t="s">
+      <c r="A4" s="61" t="s">
         <v>31</v>
       </c>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
+      <c r="B4" s="62"/>
+      <c r="C4" s="62"/>
       <c r="D4" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="E4" s="41" t="s">
+      <c r="E4" s="63" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="41"/>
-      <c r="G4" s="42" t="s">
+      <c r="F4" s="63"/>
+      <c r="G4" s="64" t="s">
         <v>46</v>
       </c>
-      <c r="H4" s="43"/>
+      <c r="H4" s="65"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="44" t="s">
+      <c r="A5" s="45" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="45"/>
-      <c r="C5" s="45"/>
+      <c r="B5" s="46"/>
+      <c r="C5" s="46"/>
       <c r="D5" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="E5" s="46" t="s">
+      <c r="E5" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="46"/>
-      <c r="G5" s="47" t="s">
+      <c r="F5" s="47"/>
+      <c r="G5" s="48" t="s">
         <v>45</v>
       </c>
-      <c r="H5" s="48"/>
+      <c r="H5" s="49"/>
     </row>
     <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="44" t="s">
+      <c r="A6" s="45" t="s">
         <v>33</v>
       </c>
-      <c r="B6" s="45"/>
-      <c r="C6" s="45"/>
+      <c r="B6" s="46"/>
+      <c r="C6" s="46"/>
       <c r="D6" s="6"/>
-      <c r="E6" s="46" t="s">
+      <c r="E6" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="F6" s="46"/>
-      <c r="G6" s="47" t="s">
+      <c r="F6" s="47"/>
+      <c r="G6" s="48" t="s">
         <v>44</v>
       </c>
-      <c r="H6" s="48"/>
+      <c r="H6" s="49"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="44" t="s">
+      <c r="A7" s="45" t="s">
         <v>34</v>
       </c>
-      <c r="B7" s="45"/>
-      <c r="C7" s="45"/>
+      <c r="B7" s="46"/>
+      <c r="C7" s="46"/>
       <c r="D7" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="E7" s="46" t="s">
+      <c r="E7" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="F7" s="46"/>
-      <c r="G7" s="47" t="s">
+      <c r="F7" s="47"/>
+      <c r="G7" s="48" t="s">
         <v>52</v>
       </c>
-      <c r="H7" s="48"/>
+      <c r="H7" s="49"/>
     </row>
     <row r="8" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="44" t="s">
+      <c r="A8" s="45" t="s">
         <v>35</v>
       </c>
-      <c r="B8" s="45"/>
-      <c r="C8" s="45"/>
+      <c r="B8" s="46"/>
+      <c r="C8" s="46"/>
       <c r="D8" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="E8" s="46" t="s">
+      <c r="E8" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="F8" s="46"/>
-      <c r="G8" s="47" t="s">
+      <c r="F8" s="47"/>
+      <c r="G8" s="48" t="s">
         <v>43</v>
       </c>
-      <c r="H8" s="48"/>
+      <c r="H8" s="49"/>
     </row>
     <row r="9" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="103" t="s">
+      <c r="A9" s="77" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="104"/>
-      <c r="C9" s="104"/>
+      <c r="B9" s="78"/>
+      <c r="C9" s="78"/>
       <c r="D9" s="21"/>
-      <c r="E9" s="105"/>
-      <c r="F9" s="105"/>
-      <c r="G9" s="106"/>
-      <c r="H9" s="107"/>
+      <c r="E9" s="79"/>
+      <c r="F9" s="79"/>
+      <c r="G9" s="80"/>
+      <c r="H9" s="81"/>
     </row>
     <row r="10" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="91" t="s">
+      <c r="A10" s="96" t="s">
         <v>37</v>
       </c>
-      <c r="B10" s="92"/>
-      <c r="C10" s="93"/>
+      <c r="B10" s="97"/>
+      <c r="C10" s="98"/>
       <c r="D10" s="10"/>
-      <c r="E10" s="41" t="s">
+      <c r="E10" s="63" t="s">
         <v>42</v>
       </c>
-      <c r="F10" s="41"/>
-      <c r="G10" s="94"/>
-      <c r="H10" s="95"/>
+      <c r="F10" s="63"/>
+      <c r="G10" s="99"/>
+      <c r="H10" s="100"/>
     </row>
     <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="31" t="s">
+      <c r="A11" s="43" t="s">
         <v>38</v>
       </c>
-      <c r="B11" s="32"/>
-      <c r="C11" s="32"/>
+      <c r="B11" s="44"/>
+      <c r="C11" s="44"/>
       <c r="D11" s="58"/>
       <c r="E11" s="59"/>
       <c r="F11" s="59"/>
@@ -2262,473 +2262,507 @@
       <c r="H11" s="60"/>
     </row>
     <row r="12" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="75"/>
-      <c r="B12" s="76"/>
-      <c r="C12" s="76"/>
-      <c r="D12" s="76"/>
+      <c r="A12" s="41"/>
+      <c r="B12" s="42"/>
+      <c r="C12" s="42"/>
+      <c r="D12" s="42"/>
       <c r="E12" s="8" t="s">
         <v>7</v>
       </c>
       <c r="F12" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="G12" s="61" t="s">
+      <c r="G12" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="H12" s="62"/>
+      <c r="H12" s="37"/>
     </row>
     <row r="13" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="100" t="s">
+      <c r="B13" s="101" t="s">
         <v>62</v>
       </c>
-      <c r="C13" s="101"/>
-      <c r="D13" s="102"/>
+      <c r="C13" s="102"/>
+      <c r="D13" s="103"/>
       <c r="E13" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F13" s="10"/>
-      <c r="G13" s="64"/>
-      <c r="H13" s="65"/>
+      <c r="G13" s="39"/>
+      <c r="H13" s="40"/>
     </row>
     <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="97" t="s">
+      <c r="B14" s="82" t="s">
         <v>63</v>
       </c>
-      <c r="C14" s="98"/>
-      <c r="D14" s="99"/>
+      <c r="C14" s="83"/>
+      <c r="D14" s="84"/>
       <c r="E14" s="7" t="s">
         <v>12</v>
       </c>
       <c r="F14" s="7"/>
-      <c r="G14" s="96"/>
-      <c r="H14" s="78"/>
+      <c r="G14" s="85"/>
+      <c r="H14" s="86"/>
     </row>
     <row r="15" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="97" t="s">
+      <c r="B15" s="82" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="98"/>
-      <c r="D15" s="99"/>
+      <c r="C15" s="83"/>
+      <c r="D15" s="84"/>
       <c r="E15" s="7" t="s">
         <v>12</v>
       </c>
       <c r="F15" s="7"/>
-      <c r="G15" s="96"/>
-      <c r="H15" s="78"/>
+      <c r="G15" s="85"/>
+      <c r="H15" s="86"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="97" t="s">
+      <c r="B16" s="82" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="98"/>
-      <c r="D16" s="99"/>
+      <c r="C16" s="83"/>
+      <c r="D16" s="84"/>
       <c r="E16" s="7" t="s">
         <v>12</v>
       </c>
       <c r="F16" s="7"/>
-      <c r="G16" s="96"/>
-      <c r="H16" s="78"/>
+      <c r="G16" s="85"/>
+      <c r="H16" s="86"/>
     </row>
     <row r="17" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="97" t="s">
+      <c r="B17" s="82" t="s">
         <v>72</v>
       </c>
-      <c r="C17" s="98"/>
-      <c r="D17" s="99"/>
+      <c r="C17" s="83"/>
+      <c r="D17" s="84"/>
       <c r="E17" s="12" t="s">
         <v>39</v>
       </c>
       <c r="F17" s="7"/>
-      <c r="G17" s="96"/>
-      <c r="H17" s="78"/>
+      <c r="G17" s="85"/>
+      <c r="H17" s="86"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="B18" s="97" t="s">
+      <c r="B18" s="82" t="s">
         <v>22</v>
       </c>
-      <c r="C18" s="98"/>
-      <c r="D18" s="99"/>
+      <c r="C18" s="83"/>
+      <c r="D18" s="84"/>
       <c r="E18" s="7" t="s">
         <v>12</v>
       </c>
       <c r="F18" s="7"/>
-      <c r="G18" s="96"/>
-      <c r="H18" s="78"/>
+      <c r="G18" s="85"/>
+      <c r="H18" s="86"/>
     </row>
     <row r="19" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="97" t="s">
+      <c r="B19" s="82" t="s">
         <v>64</v>
       </c>
-      <c r="C19" s="98"/>
-      <c r="D19" s="99"/>
+      <c r="C19" s="83"/>
+      <c r="D19" s="84"/>
       <c r="E19" s="7" t="s">
         <v>12</v>
       </c>
       <c r="F19" s="7"/>
-      <c r="G19" s="96"/>
-      <c r="H19" s="78"/>
+      <c r="G19" s="85"/>
+      <c r="H19" s="86"/>
     </row>
     <row r="20" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="B20" s="97" t="s">
+      <c r="B20" s="82" t="s">
         <v>65</v>
       </c>
-      <c r="C20" s="98"/>
-      <c r="D20" s="99"/>
+      <c r="C20" s="83"/>
+      <c r="D20" s="84"/>
       <c r="E20" s="7" t="s">
         <v>12</v>
       </c>
       <c r="F20" s="7"/>
-      <c r="G20" s="96"/>
-      <c r="H20" s="78"/>
+      <c r="G20" s="85"/>
+      <c r="H20" s="86"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="B21" s="97" t="s">
+      <c r="B21" s="82" t="s">
         <v>66</v>
       </c>
-      <c r="C21" s="98"/>
-      <c r="D21" s="99"/>
+      <c r="C21" s="83"/>
+      <c r="D21" s="84"/>
       <c r="E21" s="7"/>
       <c r="F21" s="7"/>
-      <c r="G21" s="96"/>
-      <c r="H21" s="78"/>
+      <c r="G21" s="85"/>
+      <c r="H21" s="86"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="B22" s="97" t="s">
+      <c r="B22" s="82" t="s">
         <v>67</v>
       </c>
-      <c r="C22" s="98"/>
-      <c r="D22" s="99"/>
+      <c r="C22" s="83"/>
+      <c r="D22" s="84"/>
       <c r="E22" s="7"/>
       <c r="F22" s="7"/>
-      <c r="G22" s="96"/>
-      <c r="H22" s="78"/>
+      <c r="G22" s="85"/>
+      <c r="H22" s="86"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="B23" s="97" t="s">
+      <c r="B23" s="82" t="s">
         <v>68</v>
       </c>
-      <c r="C23" s="98"/>
-      <c r="D23" s="99"/>
+      <c r="C23" s="83"/>
+      <c r="D23" s="84"/>
       <c r="E23" s="7"/>
       <c r="F23" s="7"/>
-      <c r="G23" s="96"/>
-      <c r="H23" s="78"/>
+      <c r="G23" s="85"/>
+      <c r="H23" s="86"/>
     </row>
     <row r="24" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="B24" s="97" t="s">
+      <c r="B24" s="82" t="s">
         <v>69</v>
       </c>
-      <c r="C24" s="98"/>
-      <c r="D24" s="99"/>
+      <c r="C24" s="83"/>
+      <c r="D24" s="84"/>
       <c r="E24" s="12"/>
       <c r="F24" s="7"/>
-      <c r="G24" s="96"/>
-      <c r="H24" s="78"/>
+      <c r="G24" s="85"/>
+      <c r="H24" s="86"/>
     </row>
     <row r="25" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="B25" s="97" t="s">
+      <c r="B25" s="82" t="s">
         <v>70</v>
       </c>
-      <c r="C25" s="98"/>
-      <c r="D25" s="99"/>
+      <c r="C25" s="83"/>
+      <c r="D25" s="84"/>
       <c r="F25" s="7"/>
-      <c r="G25" s="96"/>
-      <c r="H25" s="78"/>
+      <c r="G25" s="85"/>
+      <c r="H25" s="86"/>
     </row>
     <row r="26" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="B26" s="97" t="s">
+      <c r="B26" s="82" t="s">
         <v>71</v>
       </c>
-      <c r="C26" s="98"/>
-      <c r="D26" s="99"/>
+      <c r="C26" s="83"/>
+      <c r="D26" s="84"/>
       <c r="E26" s="7"/>
       <c r="F26" s="7"/>
-      <c r="G26" s="96"/>
-      <c r="H26" s="78"/>
+      <c r="G26" s="85"/>
+      <c r="H26" s="86"/>
     </row>
     <row r="27" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="B27" s="97" t="s">
+      <c r="B27" s="82" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="98"/>
-      <c r="D27" s="99"/>
+      <c r="C27" s="83"/>
+      <c r="D27" s="84"/>
       <c r="E27" s="14" t="s">
         <v>41</v>
       </c>
       <c r="F27" s="15"/>
-      <c r="G27" s="49"/>
-      <c r="H27" s="73"/>
+      <c r="G27" s="34"/>
+      <c r="H27" s="35"/>
     </row>
     <row r="28" spans="1:8" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="85" t="s">
+      <c r="A28" s="87" t="s">
         <v>73</v>
       </c>
-      <c r="B28" s="86"/>
-      <c r="C28" s="86"/>
-      <c r="D28" s="86"/>
-      <c r="E28" s="86"/>
-      <c r="F28" s="86"/>
-      <c r="G28" s="86"/>
-      <c r="H28" s="86"/>
+      <c r="B28" s="88"/>
+      <c r="C28" s="88"/>
+      <c r="D28" s="88"/>
+      <c r="E28" s="88"/>
+      <c r="F28" s="88"/>
+      <c r="G28" s="88"/>
+      <c r="H28" s="88"/>
     </row>
     <row r="29" spans="1:8" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="79" t="s">
+      <c r="A29" s="89" t="s">
         <v>74</v>
       </c>
-      <c r="B29" s="80"/>
+      <c r="B29" s="90"/>
       <c r="C29" s="23" t="s">
         <v>75</v>
       </c>
       <c r="D29" s="23" t="s">
         <v>76</v>
       </c>
-      <c r="E29" s="79" t="s">
+      <c r="E29" s="89" t="s">
         <v>77</v>
       </c>
-      <c r="F29" s="80"/>
-      <c r="G29" s="79" t="s">
+      <c r="F29" s="90"/>
+      <c r="G29" s="89" t="s">
         <v>78</v>
       </c>
-      <c r="H29" s="80"/>
+      <c r="H29" s="90"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="87">
+      <c r="A30" s="91">
         <v>0</v>
       </c>
-      <c r="B30" s="88"/>
+      <c r="B30" s="92"/>
       <c r="C30" s="24"/>
       <c r="D30" s="24"/>
-      <c r="E30" s="89"/>
-      <c r="F30" s="90"/>
-      <c r="G30" s="77"/>
-      <c r="H30" s="78"/>
+      <c r="E30" s="93"/>
+      <c r="F30" s="94"/>
+      <c r="G30" s="95"/>
+      <c r="H30" s="86"/>
     </row>
     <row r="31" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="81">
+      <c r="A31" s="104">
         <v>5</v>
       </c>
-      <c r="B31" s="82"/>
+      <c r="B31" s="105"/>
       <c r="C31" s="25"/>
       <c r="D31" s="25"/>
-      <c r="E31" s="77"/>
-      <c r="F31" s="78"/>
-      <c r="G31" s="77"/>
-      <c r="H31" s="78"/>
+      <c r="E31" s="95"/>
+      <c r="F31" s="86"/>
+      <c r="G31" s="95"/>
+      <c r="H31" s="86"/>
     </row>
     <row r="32" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="81">
+      <c r="A32" s="104">
         <v>25</v>
       </c>
-      <c r="B32" s="82"/>
+      <c r="B32" s="105"/>
       <c r="C32" s="25"/>
       <c r="D32" s="25"/>
-      <c r="E32" s="77"/>
-      <c r="F32" s="78"/>
-      <c r="G32" s="77"/>
-      <c r="H32" s="78"/>
+      <c r="E32" s="95"/>
+      <c r="F32" s="86"/>
+      <c r="G32" s="95"/>
+      <c r="H32" s="86"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="81">
+      <c r="A33" s="104">
         <v>50</v>
       </c>
-      <c r="B33" s="82"/>
+      <c r="B33" s="105"/>
       <c r="C33" s="25"/>
       <c r="D33" s="25"/>
-      <c r="E33" s="77"/>
-      <c r="F33" s="78"/>
-      <c r="G33" s="77"/>
-      <c r="H33" s="78"/>
+      <c r="E33" s="95"/>
+      <c r="F33" s="86"/>
+      <c r="G33" s="95"/>
+      <c r="H33" s="86"/>
     </row>
     <row r="34" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="81">
+      <c r="A34" s="104">
         <v>75</v>
       </c>
-      <c r="B34" s="82"/>
+      <c r="B34" s="105"/>
       <c r="C34" s="25"/>
       <c r="D34" s="25"/>
-      <c r="E34" s="77"/>
-      <c r="F34" s="78"/>
-      <c r="G34" s="77"/>
-      <c r="H34" s="78"/>
+      <c r="E34" s="95"/>
+      <c r="F34" s="86"/>
+      <c r="G34" s="95"/>
+      <c r="H34" s="86"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="81">
+      <c r="A35" s="104">
         <v>95</v>
       </c>
-      <c r="B35" s="82"/>
+      <c r="B35" s="105"/>
       <c r="C35" s="25"/>
       <c r="D35" s="25"/>
-      <c r="E35" s="77"/>
-      <c r="F35" s="78"/>
-      <c r="G35" s="77"/>
-      <c r="H35" s="78"/>
+      <c r="E35" s="95"/>
+      <c r="F35" s="86"/>
+      <c r="G35" s="95"/>
+      <c r="H35" s="86"/>
     </row>
     <row r="36" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="81">
+      <c r="A36" s="104">
         <v>100</v>
       </c>
-      <c r="B36" s="82"/>
+      <c r="B36" s="105"/>
       <c r="C36" s="25"/>
       <c r="D36" s="25"/>
-      <c r="E36" s="77"/>
-      <c r="F36" s="78"/>
-      <c r="G36" s="77"/>
-      <c r="H36" s="78"/>
+      <c r="E36" s="95"/>
+      <c r="F36" s="86"/>
+      <c r="G36" s="95"/>
+      <c r="H36" s="86"/>
     </row>
     <row r="37" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="81">
+      <c r="A37" s="104">
         <v>95</v>
       </c>
-      <c r="B37" s="82"/>
+      <c r="B37" s="105"/>
       <c r="C37" s="25"/>
       <c r="D37" s="25"/>
-      <c r="E37" s="77"/>
-      <c r="F37" s="78"/>
-      <c r="G37" s="77"/>
-      <c r="H37" s="78"/>
+      <c r="E37" s="95"/>
+      <c r="F37" s="86"/>
+      <c r="G37" s="95"/>
+      <c r="H37" s="86"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="81">
+      <c r="A38" s="104">
         <v>75</v>
       </c>
-      <c r="B38" s="82"/>
+      <c r="B38" s="105"/>
       <c r="C38" s="25"/>
       <c r="D38" s="25"/>
-      <c r="E38" s="77"/>
-      <c r="F38" s="78"/>
-      <c r="G38" s="77"/>
-      <c r="H38" s="78"/>
+      <c r="E38" s="95"/>
+      <c r="F38" s="86"/>
+      <c r="G38" s="95"/>
+      <c r="H38" s="86"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="81">
+      <c r="A39" s="104">
         <v>50</v>
       </c>
-      <c r="B39" s="82"/>
+      <c r="B39" s="105"/>
       <c r="C39" s="25"/>
       <c r="D39" s="25"/>
-      <c r="E39" s="77"/>
-      <c r="F39" s="78"/>
-      <c r="G39" s="77"/>
-      <c r="H39" s="78"/>
+      <c r="E39" s="95"/>
+      <c r="F39" s="86"/>
+      <c r="G39" s="95"/>
+      <c r="H39" s="86"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="81">
+      <c r="A40" s="104">
         <v>25</v>
       </c>
-      <c r="B40" s="82"/>
+      <c r="B40" s="105"/>
       <c r="C40" s="25"/>
       <c r="D40" s="25"/>
-      <c r="E40" s="77"/>
-      <c r="F40" s="78"/>
-      <c r="G40" s="77"/>
-      <c r="H40" s="78"/>
+      <c r="E40" s="95"/>
+      <c r="F40" s="86"/>
+      <c r="G40" s="95"/>
+      <c r="H40" s="86"/>
     </row>
     <row r="41" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="81">
+      <c r="A41" s="104">
         <v>5</v>
       </c>
-      <c r="B41" s="82"/>
+      <c r="B41" s="105"/>
       <c r="C41" s="25"/>
       <c r="D41" s="25"/>
-      <c r="E41" s="77"/>
-      <c r="F41" s="78"/>
-      <c r="G41" s="77"/>
-      <c r="H41" s="78"/>
+      <c r="E41" s="95"/>
+      <c r="F41" s="86"/>
+      <c r="G41" s="95"/>
+      <c r="H41" s="86"/>
     </row>
     <row r="42" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="83">
+      <c r="A42" s="106">
         <v>0</v>
       </c>
-      <c r="B42" s="84"/>
+      <c r="B42" s="107"/>
       <c r="C42" s="25"/>
       <c r="D42" s="25"/>
-      <c r="E42" s="77"/>
-      <c r="F42" s="78"/>
-      <c r="G42" s="77"/>
-      <c r="H42" s="78"/>
+      <c r="E42" s="95"/>
+      <c r="F42" s="86"/>
+      <c r="G42" s="95"/>
+      <c r="H42" s="86"/>
     </row>
     <row r="43" spans="1:8" s="18" customFormat="1" ht="92.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="69" t="s">
+      <c r="A43" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="B43" s="70"/>
-      <c r="C43" s="70"/>
-      <c r="D43" s="70"/>
-      <c r="E43" s="70"/>
-      <c r="F43" s="70"/>
-      <c r="G43" s="70"/>
-      <c r="H43" s="71"/>
+      <c r="B43" s="31"/>
+      <c r="C43" s="31"/>
+      <c r="D43" s="31"/>
+      <c r="E43" s="31"/>
+      <c r="F43" s="31"/>
+      <c r="G43" s="31"/>
+      <c r="H43" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="104">
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="G41:H41"/>
+    <mergeCell ref="G42:H42"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="G35:H35"/>
+    <mergeCell ref="G36:H36"/>
+    <mergeCell ref="G37:H37"/>
+    <mergeCell ref="G38:H38"/>
+    <mergeCell ref="G39:H39"/>
+    <mergeCell ref="G40:H40"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="E39:F39"/>
+    <mergeCell ref="E40:F40"/>
+    <mergeCell ref="E41:F41"/>
+    <mergeCell ref="E42:F42"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="G33:H33"/>
+    <mergeCell ref="G34:H34"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="D11:H11"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="A12:D12"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="G14:H14"/>
     <mergeCell ref="A43:H43"/>
     <mergeCell ref="B16:D16"/>
     <mergeCell ref="B17:D17"/>
@@ -2753,63 +2787,29 @@
     <mergeCell ref="G20:H20"/>
     <mergeCell ref="A28:H28"/>
     <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="A10:C10"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="A11:C11"/>
-    <mergeCell ref="D11:H11"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="A12:D12"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="G41:H41"/>
-    <mergeCell ref="G42:H42"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="G35:H35"/>
-    <mergeCell ref="G36:H36"/>
-    <mergeCell ref="G37:H37"/>
-    <mergeCell ref="G38:H38"/>
-    <mergeCell ref="G39:H39"/>
-    <mergeCell ref="G40:H40"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="E39:F39"/>
-    <mergeCell ref="E40:F40"/>
-    <mergeCell ref="E41:F41"/>
-    <mergeCell ref="E42:F42"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="G33:H33"/>
-    <mergeCell ref="G34:H34"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G4:H4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2836,30 +2836,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="74" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="38"/>
+      <c r="B1" s="75"/>
+      <c r="C1" s="75"/>
+      <c r="D1" s="75"/>
+      <c r="E1" s="75"/>
+      <c r="F1" s="75"/>
+      <c r="G1" s="75"/>
+      <c r="H1" s="76"/>
     </row>
     <row r="2" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="66" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="27"/>
+      <c r="B2" s="67"/>
       <c r="C2" s="16">
         <v>1</v>
       </c>
-      <c r="D2" s="28" t="s">
+      <c r="D2" s="68" t="s">
         <v>82</v>
       </c>
-      <c r="E2" s="29"/>
-      <c r="F2" s="30"/>
+      <c r="E2" s="69"/>
+      <c r="F2" s="70"/>
       <c r="G2" s="19" t="s">
         <v>28</v>
       </c>
@@ -2868,18 +2868,18 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="31" t="s">
+      <c r="A3" s="43" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="32"/>
+      <c r="B3" s="44"/>
       <c r="C3" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="33" t="s">
+      <c r="D3" s="71" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="34"/>
-      <c r="F3" s="35"/>
+      <c r="E3" s="72"/>
+      <c r="F3" s="73"/>
       <c r="G3" s="20" t="s">
         <v>53</v>
       </c>
@@ -2888,102 +2888,102 @@
       </c>
     </row>
     <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="39" t="s">
+      <c r="A4" s="61" t="s">
         <v>31</v>
       </c>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
+      <c r="B4" s="62"/>
+      <c r="C4" s="62"/>
       <c r="D4" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="E4" s="41" t="s">
+      <c r="E4" s="63" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="41"/>
-      <c r="G4" s="42" t="s">
+      <c r="F4" s="63"/>
+      <c r="G4" s="64" t="s">
         <v>46</v>
       </c>
-      <c r="H4" s="43"/>
+      <c r="H4" s="65"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="44" t="s">
+      <c r="A5" s="45" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="45"/>
-      <c r="C5" s="45"/>
+      <c r="B5" s="46"/>
+      <c r="C5" s="46"/>
       <c r="D5" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="E5" s="46" t="s">
+      <c r="E5" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="46"/>
-      <c r="G5" s="47" t="s">
+      <c r="F5" s="47"/>
+      <c r="G5" s="48" t="s">
         <v>45</v>
       </c>
-      <c r="H5" s="48"/>
+      <c r="H5" s="49"/>
     </row>
     <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="44" t="s">
+      <c r="A6" s="45" t="s">
         <v>33</v>
       </c>
-      <c r="B6" s="45"/>
-      <c r="C6" s="45"/>
+      <c r="B6" s="46"/>
+      <c r="C6" s="46"/>
       <c r="D6" s="6"/>
-      <c r="E6" s="46" t="s">
+      <c r="E6" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="F6" s="46"/>
-      <c r="G6" s="47" t="s">
+      <c r="F6" s="47"/>
+      <c r="G6" s="48" t="s">
         <v>44</v>
       </c>
-      <c r="H6" s="48"/>
+      <c r="H6" s="49"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="44" t="s">
+      <c r="A7" s="45" t="s">
         <v>34</v>
       </c>
-      <c r="B7" s="45"/>
-      <c r="C7" s="45"/>
+      <c r="B7" s="46"/>
+      <c r="C7" s="46"/>
       <c r="D7" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="E7" s="46" t="s">
+      <c r="E7" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="F7" s="46"/>
-      <c r="G7" s="47" t="s">
+      <c r="F7" s="47"/>
+      <c r="G7" s="48" t="s">
         <v>52</v>
       </c>
-      <c r="H7" s="48"/>
+      <c r="H7" s="49"/>
     </row>
     <row r="8" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="44" t="s">
+      <c r="A8" s="45" t="s">
         <v>35</v>
       </c>
-      <c r="B8" s="45"/>
-      <c r="C8" s="45"/>
+      <c r="B8" s="46"/>
+      <c r="C8" s="46"/>
       <c r="D8" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="E8" s="46" t="s">
+      <c r="E8" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="F8" s="46"/>
-      <c r="G8" s="47" t="s">
+      <c r="F8" s="47"/>
+      <c r="G8" s="48" t="s">
         <v>43</v>
       </c>
-      <c r="H8" s="48"/>
+      <c r="H8" s="49"/>
     </row>
     <row r="9" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="31" t="s">
+      <c r="A9" s="43" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="32"/>
-      <c r="C9" s="32"/>
+      <c r="B9" s="44"/>
+      <c r="C9" s="44"/>
       <c r="D9" s="2"/>
-      <c r="E9" s="49"/>
-      <c r="F9" s="49"/>
+      <c r="E9" s="34"/>
+      <c r="F9" s="34"/>
       <c r="G9" s="50"/>
       <c r="H9" s="51"/>
     </row>
@@ -3002,11 +3002,11 @@
       <c r="H10" s="57"/>
     </row>
     <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="31" t="s">
+      <c r="A11" s="43" t="s">
         <v>38</v>
       </c>
-      <c r="B11" s="32"/>
-      <c r="C11" s="32"/>
+      <c r="B11" s="44"/>
+      <c r="C11" s="44"/>
       <c r="D11" s="58"/>
       <c r="E11" s="59"/>
       <c r="F11" s="59"/>
@@ -3014,115 +3014,148 @@
       <c r="H11" s="60"/>
     </row>
     <row r="12" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="75"/>
-      <c r="B12" s="76"/>
-      <c r="C12" s="76"/>
-      <c r="D12" s="76"/>
+      <c r="A12" s="41"/>
+      <c r="B12" s="42"/>
+      <c r="C12" s="42"/>
+      <c r="D12" s="42"/>
       <c r="E12" s="8" t="s">
         <v>7</v>
       </c>
       <c r="F12" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="G12" s="61" t="s">
+      <c r="G12" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="H12" s="62"/>
+      <c r="H12" s="37"/>
     </row>
     <row r="13" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="63" t="s">
+      <c r="B13" s="38" t="s">
         <v>62</v>
       </c>
-      <c r="C13" s="63"/>
-      <c r="D13" s="63"/>
+      <c r="C13" s="38"/>
+      <c r="D13" s="38"/>
       <c r="E13" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F13" s="10"/>
-      <c r="G13" s="64"/>
-      <c r="H13" s="65"/>
+      <c r="G13" s="39"/>
+      <c r="H13" s="40"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="66" t="s">
+      <c r="B14" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="66"/>
-      <c r="D14" s="66"/>
+      <c r="C14" s="26"/>
+      <c r="D14" s="26"/>
       <c r="E14" s="7" t="s">
         <v>12</v>
       </c>
       <c r="F14" s="7"/>
-      <c r="G14" s="67"/>
-      <c r="H14" s="68"/>
+      <c r="G14" s="27"/>
+      <c r="H14" s="28"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="74" t="s">
+      <c r="B15" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="C15" s="74"/>
-      <c r="D15" s="74"/>
+      <c r="C15" s="29"/>
+      <c r="D15" s="29"/>
       <c r="E15" s="12" t="s">
         <v>40</v>
       </c>
       <c r="F15" s="7"/>
-      <c r="G15" s="67"/>
-      <c r="H15" s="68"/>
+      <c r="G15" s="27"/>
+      <c r="H15" s="28"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="66" t="s">
+      <c r="B16" s="26" t="s">
         <v>80</v>
       </c>
-      <c r="C16" s="66"/>
-      <c r="D16" s="66"/>
+      <c r="C16" s="26"/>
+      <c r="D16" s="26"/>
       <c r="E16" s="12" t="s">
         <v>39</v>
       </c>
       <c r="F16" s="7"/>
-      <c r="G16" s="67"/>
-      <c r="H16" s="68"/>
+      <c r="G16" s="27"/>
+      <c r="H16" s="28"/>
     </row>
     <row r="17" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="B17" s="66" t="s">
+      <c r="B17" s="26" t="s">
         <v>81</v>
       </c>
-      <c r="C17" s="66"/>
-      <c r="D17" s="66"/>
+      <c r="C17" s="26"/>
+      <c r="D17" s="26"/>
       <c r="E17" s="7" t="s">
         <v>12</v>
       </c>
       <c r="F17" s="7"/>
-      <c r="G17" s="67"/>
-      <c r="H17" s="68"/>
+      <c r="G17" s="27"/>
+      <c r="H17" s="28"/>
     </row>
     <row r="18" spans="1:8" s="18" customFormat="1" ht="92.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="69" t="s">
+      <c r="A18" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="B18" s="70"/>
-      <c r="C18" s="70"/>
-      <c r="D18" s="70"/>
-      <c r="E18" s="70"/>
-      <c r="F18" s="70"/>
-      <c r="G18" s="70"/>
-      <c r="H18" s="71"/>
+      <c r="B18" s="31"/>
+      <c r="C18" s="31"/>
+      <c r="D18" s="31"/>
+      <c r="E18" s="31"/>
+      <c r="F18" s="31"/>
+      <c r="G18" s="31"/>
+      <c r="H18" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="41">
+    <mergeCell ref="A18:H18"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="D11:H11"/>
+    <mergeCell ref="A12:D12"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="G6:H6"/>
     <mergeCell ref="A4:C4"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="G4:H4"/>
@@ -3131,39 +3164,6 @@
     <mergeCell ref="D2:F2"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="D3:F3"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="A10:C10"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="A11:C11"/>
-    <mergeCell ref="D11:H11"/>
-    <mergeCell ref="A12:D12"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="A18:H18"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="G17:H17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>